<commit_message>
Added town listing and styles.
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\Documents\Ads-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7815"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11985"/>
   </bookViews>
   <sheets>
     <sheet name="JS-SPA-Self-Evaluation-Protocol" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -399,10 +399,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,11 +753,11 @@
       <c r="B7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="21" t="s">
+      <c r="C7" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
@@ -1119,7 +1119,9 @@
       <c r="B39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="7"/>
+      <c r="C39" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D39" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added edit and delete category.
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1161,7 +1161,9 @@
       <c r="B43" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C43" s="7"/>
+      <c r="C43" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D43" s="7" t="s">
         <v>28</v>
       </c>
@@ -1171,7 +1173,9 @@
       <c r="B44" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="7"/>
+      <c r="C44" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D44" s="7" t="s">
         <v>28</v>
       </c>
@@ -1201,7 +1205,9 @@
       <c r="B47" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C47" s="7"/>
+      <c r="C47" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D47" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added create new town.
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1185,7 +1185,9 @@
       <c r="B45" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="7"/>
+      <c r="C45" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D45" s="7" t="s">
         <v>28</v>
       </c>
@@ -1195,7 +1197,9 @@
       <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C46" s="7"/>
+      <c r="C46" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D46" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added town edit and delete.
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -689,7 +689,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C48" sqref="C48"/>
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1221,7 +1221,9 @@
       <c r="B48" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C48" s="7"/>
+      <c r="C48" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D48" s="7" t="s">
         <v>28</v>
       </c>
@@ -1231,7 +1233,9 @@
       <c r="B49" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C49" s="7"/>
+      <c r="C49" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D49" s="7" t="s">
         <v>28</v>
       </c>
@@ -1241,7 +1245,9 @@
       <c r="B50" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C50" s="7"/>
+      <c r="C50" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D50" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added admin edit user and password change.
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="61">
   <si>
     <t>Days Commit in GitHub</t>
   </si>
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J39" sqref="J39"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1131,7 +1131,9 @@
       <c r="B40" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="7"/>
+      <c r="C40" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D40" s="7" t="s">
         <v>28</v>
       </c>
@@ -1141,7 +1143,9 @@
       <c r="B41" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="7"/>
+      <c r="C41" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
       </c>
@@ -1151,7 +1155,9 @@
       <c r="B42" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="7"/>
+      <c r="C42" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="D42" s="7" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Updated with some minor changes in the header title controller.
</commit_message>
<xml_diff>
--- a/JS-SPA-Self-Evaluation-Protocol.xlsx
+++ b/JS-SPA-Self-Evaluation-Protocol.xlsx
@@ -673,7 +673,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -684,7 +684,7 @@
   <dimension ref="B2:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -771,7 +771,7 @@
         <v>1</v>
       </c>
       <c r="C9" s="6">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D9" s="12" t="s">
         <v>56</v>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="C51" s="11">
         <f>SUM(C6:C50)</f>
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="D51" s="11">
         <v>430</v>

</xml_diff>